<commit_message>
working on gurobi like implementation
</commit_message>
<xml_diff>
--- a/New-Implementation/Data/simple-data.xlsx
+++ b/New-Implementation/Data/simple-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Projects\UOttawa-Dynamic-Knapsack-Problem-Python\New-Implementation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FEB9F6-D93C-4145-B9E2-7F9B8D860ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1748D8-4807-4788-AC54-D318181D676E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2310" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Indices Data" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="45">
   <si>
     <t>Time Horizon (t)</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>C2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1297,8 +1300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1376,7 +1379,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="10">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="2"/>
@@ -1965,8 +1968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AMJ222"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2072,7 +2075,7 @@
         <v>9</v>
       </c>
       <c r="G3" s="19">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H3" s="16">
         <v>1</v>
@@ -2109,7 +2112,7 @@
         <v>9</v>
       </c>
       <c r="G4" s="19">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H4" s="16">
         <v>1</v>
@@ -2127,7 +2130,7 @@
         <v>9</v>
       </c>
       <c r="M4" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -2146,7 +2149,7 @@
         <v>9</v>
       </c>
       <c r="G5" s="19">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H5" s="16">
         <v>1</v>
@@ -2164,7 +2167,7 @@
         <v>9</v>
       </c>
       <c r="M5" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2183,7 +2186,7 @@
         <v>9</v>
       </c>
       <c r="G6" s="19">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H6" s="16">
         <v>1</v>
@@ -2201,7 +2204,7 @@
         <v>9</v>
       </c>
       <c r="M6" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -2220,7 +2223,7 @@
         <v>9</v>
       </c>
       <c r="G7" s="19">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H7" s="16">
         <v>1</v>
@@ -2238,7 +2241,7 @@
         <v>9</v>
       </c>
       <c r="M7" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -2312,7 +2315,7 @@
         <v>9</v>
       </c>
       <c r="M9" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -2349,7 +2352,7 @@
         <v>9</v>
       </c>
       <c r="M10" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -2368,7 +2371,7 @@
         <v>9</v>
       </c>
       <c r="G11" s="19">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H11" s="16">
         <v>2</v>
@@ -2386,7 +2389,7 @@
         <v>9</v>
       </c>
       <c r="M11" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -2405,7 +2408,7 @@
         <v>9</v>
       </c>
       <c r="G12" s="19">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H12" s="16">
         <v>2</v>
@@ -2423,7 +2426,7 @@
         <v>9</v>
       </c>
       <c r="M12" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -2477,7 +2480,7 @@
         <v>9</v>
       </c>
       <c r="M14" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -2499,7 +2502,7 @@
         <v>9</v>
       </c>
       <c r="M15" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -2521,10 +2524,10 @@
         <v>9</v>
       </c>
       <c r="M16" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
       <c r="B17" s="22"/>
       <c r="C17" s="18"/>
@@ -2548,10 +2551,10 @@
         <v>9</v>
       </c>
       <c r="M17" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
       <c r="B18" s="22"/>
       <c r="C18" s="18"/>
@@ -2578,7 +2581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="18"/>
@@ -2602,10 +2605,10 @@
         <v>9</v>
       </c>
       <c r="M19" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="18"/>
@@ -2629,10 +2632,10 @@
         <v>9</v>
       </c>
       <c r="M20" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="22"/>
       <c r="B21" s="22"/>
       <c r="C21" s="18"/>
@@ -2656,10 +2659,10 @@
         <v>9</v>
       </c>
       <c r="M21" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="22"/>
       <c r="B22" s="22"/>
       <c r="C22" s="18"/>
@@ -2683,10 +2686,10 @@
         <v>9</v>
       </c>
       <c r="M22" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
@@ -2710,8 +2713,11 @@
       <c r="M23" s="21">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="AC23" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
       <c r="E24" s="18"/>
@@ -2736,7 +2742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="H25" s="16">
         <v>1</v>
       </c>
@@ -2756,7 +2762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="H26" s="16">
         <v>1</v>
       </c>
@@ -2776,7 +2782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="H27" s="16">
         <v>1</v>
       </c>
@@ -2796,7 +2802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="H28" s="16">
         <v>2</v>
       </c>
@@ -2816,7 +2822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="H29" s="16">
         <v>2</v>
       </c>
@@ -2836,7 +2842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="H30" s="16">
         <v>2</v>
       </c>
@@ -2856,7 +2862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="H31" s="16">
         <v>2</v>
       </c>
@@ -2876,7 +2882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="H32" s="16">
         <v>2</v>
       </c>
@@ -2933,7 +2939,7 @@
         <v>9</v>
       </c>
       <c r="M34" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="8:13" x14ac:dyDescent="0.25">
@@ -2953,7 +2959,7 @@
         <v>9</v>
       </c>
       <c r="M35" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="8:13" x14ac:dyDescent="0.25">
@@ -2973,7 +2979,7 @@
         <v>9</v>
       </c>
       <c r="M36" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="8:13" x14ac:dyDescent="0.25">
@@ -2993,7 +2999,7 @@
         <v>9</v>
       </c>
       <c r="M37" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="8:13" x14ac:dyDescent="0.25">
@@ -3033,7 +3039,7 @@
         <v>9</v>
       </c>
       <c r="M39" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="8:13" x14ac:dyDescent="0.25">
@@ -3053,7 +3059,7 @@
         <v>9</v>
       </c>
       <c r="M40" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="8:13" x14ac:dyDescent="0.25">
@@ -3073,7 +3079,7 @@
         <v>9</v>
       </c>
       <c r="M41" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="8:13" x14ac:dyDescent="0.25">
@@ -3093,7 +3099,7 @@
         <v>9</v>
       </c>
       <c r="M42" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="8:13" x14ac:dyDescent="0.25">

</xml_diff>